<commit_message>
Convert the query to its representation of the reduced dimension
</commit_message>
<xml_diff>
--- a/tfidf/tfidf_result.xlsx
+++ b/tfidf/tfidf_result.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SingSing\Documents\GitHub\SVD-and-Truncated-SVD\tfidf\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0091380F-D056-4B69-A2F8-D61AB1FB8FA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2565" yWindow="2557" windowWidth="14947" windowHeight="9758" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="tfidf" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>frequent</t>
   </si>
@@ -62,17 +56,20 @@
   </si>
   <si>
     <t>doc_4.txt</t>
+  </si>
+  <si>
+    <t>query.txt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -80,15 +77,8 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -134,23 +124,15 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -192,7 +174,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -224,27 +206,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -276,24 +240,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -469,19 +415,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -513,7 +454,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -521,16 +462,16 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>5.7536414490356173E-2</v>
+        <v>0.1021651247531982</v>
       </c>
       <c r="D2">
-        <v>0.2772588722239781</v>
+        <v>0.3218875824868201</v>
       </c>
       <c r="E2">
-        <v>0.2772588722239781</v>
+        <v>0.3218875824868201</v>
       </c>
       <c r="F2">
-        <v>5.7536414490356173E-2</v>
+        <v>0.04462871026284196</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -539,7 +480,7 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0.13862943611198911</v>
+        <v>0.183258146374831</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -548,15 +489,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B3">
-        <v>0.34657359027997259</v>
+        <v>0.4023594781085251</v>
       </c>
       <c r="C3">
-        <v>7.1920518112945211E-2</v>
+        <v>0.1277064059414977</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -568,7 +509,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0.17328679513998629</v>
+        <v>0.1277064059414977</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -577,13 +518,13 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0.17328679513998629</v>
+        <v>0.1277064059414977</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -591,7 +532,7 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>5.7536414490356173E-2</v>
+        <v>0.1021651247531982</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -600,10 +541,10 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.11507282898071231</v>
+        <v>0.08925742052568392</v>
       </c>
       <c r="G4">
-        <v>0.13862943611198911</v>
+        <v>0.1021651247531982</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -612,13 +553,13 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0.13862943611198911</v>
+        <v>0.1021651247531982</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -635,27 +576,60 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>5.7536414490356173E-2</v>
+        <v>0.04462871026284196</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>0.2772588722239781</v>
+        <v>0.3218875824868201</v>
       </c>
       <c r="I5">
-        <v>0.2772588722239781</v>
+        <v>0.3665162927496621</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5">
-        <v>0.2772588722239781</v>
+        <v>0.3218875824868201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0.07438118377140325</v>
+      </c>
+      <c r="G6">
+        <v>0.1702752079219969</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0.1702752079219969</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>